<commit_message>
updated pin allocation (added current sense OCD pins), worked on schematic
</commit_message>
<xml_diff>
--- a/Design Docs/STM32 Pin Allocation.xlsx
+++ b/Design Docs/STM32 Pin Allocation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901B0789-C5C9-4588-A047-34E3384B7F28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B97A0-EE11-4B1C-9DED-E82C3A89A22B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="354" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="203">
   <si>
     <t>PC10</t>
   </si>
@@ -529,27 +529,6 @@
     <t>Relay Control 3 (GPIO)</t>
   </si>
   <si>
-    <t>Current Sense 1 (ADC)</t>
-  </si>
-  <si>
-    <t>Temp Sense 12? (ADC)</t>
-  </si>
-  <si>
-    <t>Current Sense 2 (ADC)</t>
-  </si>
-  <si>
-    <t>Current Sense 3 (ADC)</t>
-  </si>
-  <si>
-    <t>Current Sense 4 (ADC)</t>
-  </si>
-  <si>
-    <t>Current Sense 5 (ADC)</t>
-  </si>
-  <si>
-    <t>Current Sense 6 (ADC)</t>
-  </si>
-  <si>
     <t>Voltage Sense 3 (ADC)</t>
   </si>
   <si>
@@ -599,6 +578,57 @@
   </si>
   <si>
     <t>5V In from Buck (POWER)</t>
+  </si>
+  <si>
+    <t>Input Current Sense 1 (ADC)</t>
+  </si>
+  <si>
+    <t>Input Current Sense 2 (ADC)</t>
+  </si>
+  <si>
+    <t>Input Current Sense 3 (ADC)</t>
+  </si>
+  <si>
+    <t>Output Current Sense 1 (ADC)</t>
+  </si>
+  <si>
+    <t>Output Current Sense 2 (ADC)</t>
+  </si>
+  <si>
+    <t>Output Current Sense 3 (ADC)</t>
+  </si>
+  <si>
+    <t>Generic LED 1 (GPIO)</t>
+  </si>
+  <si>
+    <t>I_IN_1_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>I_IN_2_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>I_IN_3_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>I_OUT_1_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>I_OUT_2_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>I_OUT_3_OCD (GPIO)</t>
+  </si>
+  <si>
+    <t>USART1_CK (NC)</t>
+  </si>
+  <si>
+    <t>USART1_TX (NC)</t>
+  </si>
+  <si>
+    <t>USART1_RX (NC)</t>
+  </si>
+  <si>
+    <t>JTAG (NC)</t>
   </si>
 </sst>
 </file>
@@ -672,7 +702,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -690,6 +727,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
@@ -697,6 +769,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
@@ -704,6 +818,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -726,6 +854,167 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1014,8 +1303,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1026,7 +1315,7 @@
     <col min="4" max="4" width="14.59765625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.86328125" style="4" customWidth="1"/>
     <col min="8" max="9" width="11.46484375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.59765625" style="4" customWidth="1"/>
     <col min="11" max="11" width="13" style="4" bestFit="1" customWidth="1"/>
@@ -1034,7 +1323,7 @@
     <col min="13" max="13" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.53125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.9296875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="13.86328125" customWidth="1"/>
+    <col min="16" max="16" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
@@ -1103,7 +1392,7 @@
         <v>89</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1126,10 +1415,10 @@
         <v>89</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1149,7 +1438,7 @@
         <v>89</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1172,7 +1461,7 @@
         <v>89</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -1195,7 +1484,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1221,7 +1510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1240,7 +1529,9 @@
       <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="4">
@@ -1262,7 +1553,7 @@
         <v>89</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -1331,7 +1622,7 @@
         <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1354,7 +1645,7 @@
         <v>70</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="57" x14ac:dyDescent="0.45">
@@ -1423,7 +1714,7 @@
         <v>70</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1492,7 +1783,7 @@
         <v>70</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -1584,7 +1875,7 @@
         <v>163</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -1630,7 +1921,7 @@
         <v>89</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -1652,7 +1943,9 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="4">
@@ -1674,7 +1967,7 @@
         <v>70</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="57" x14ac:dyDescent="0.45">
@@ -1720,7 +2013,7 @@
         <v>89</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -1742,7 +2035,9 @@
       <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="4">
@@ -1764,7 +2059,7 @@
         <v>70</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="57" x14ac:dyDescent="0.45">
@@ -1787,7 +2082,7 @@
         <v>73</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1809,6 +2104,9 @@
       <c r="O17" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P17" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="18" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
@@ -1829,7 +2127,9 @@
       <c r="F18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="4">
@@ -1850,6 +2150,9 @@
       <c r="O18" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P18" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
@@ -1871,7 +2174,7 @@
         <v>74</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1893,8 +2196,11 @@
       <c r="O19" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P19" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1914,7 +2220,7 @@
         <v>70</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1936,6 +2242,9 @@
       <c r="O20" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P20" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
@@ -1957,7 +2266,7 @@
         <v>70</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1980,7 +2289,7 @@
         <v>70</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
@@ -2002,7 +2311,9 @@
       <c r="F22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="4">
@@ -2023,8 +2334,11 @@
       <c r="O22" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P22" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2044,7 +2358,7 @@
         <v>70</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -2066,6 +2380,9 @@
       <c r="O23" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P23" s="2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -2109,6 +2426,9 @@
       <c r="O24" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P24" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="25" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
@@ -2130,7 +2450,7 @@
         <v>71</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -2153,7 +2473,7 @@
         <v>70</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -2284,6 +2604,9 @@
       <c r="O28" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P28" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="57" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
@@ -2305,7 +2628,7 @@
         <v>70</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -2391,7 +2714,7 @@
         <v>70</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -2456,6 +2779,9 @@
       <c r="O32" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P32" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="33" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
@@ -2477,7 +2803,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2500,7 +2826,7 @@
         <v>121</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -2545,6 +2871,9 @@
       <c r="O34" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="P34" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="35" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
@@ -2566,7 +2895,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2589,7 +2918,7 @@
         <v>70</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -2612,7 +2941,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2658,7 +2987,7 @@
         <v>70</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2704,7 +3033,7 @@
         <v>70</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2750,7 +3079,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2778,30 +3107,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G39 P2:P39">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="(CAN)">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="(POWER)">
+      <formula>NOT(ISERROR(SEARCH("(POWER)",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="(CAN)">
       <formula>NOT(ISERROR(SEARCH("(CAN)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="(SPI)">
+    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="(SPI)">
       <formula>NOT(ISERROR(SEARCH("(SPI)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="(ADC)">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="(ADC)">
       <formula>NOT(ISERROR(SEARCH("(ADC)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="4" priority="11">
+    <cfRule type="containsBlanks" dxfId="18" priority="12">
       <formula>LEN(TRIM(G2))=0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="(POWER)">
-      <formula>NOT(ISERROR(SEARCH("(POWER)",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F39 K2:O39">
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G39 I2:P39">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
-      <formula>"NC"</formula>
+  <conditionalFormatting sqref="A2:P39">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="NC">
+      <formula>NOT(ISERROR(SEARCH("NC",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2810,7 +3139,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{8501BA9A-327E-4BFA-BA01-860A8162A1FE}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{8501BA9A-327E-4BFA-BA01-860A8162A1FE}">
             <xm:f>NOT(ISERROR(SEARCH("(GPIO)",G2)))</xm:f>
             <xm:f>"(GPIO)"</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
added TVS diodes, optimized pin allocation, finished STM schematic connections
</commit_message>
<xml_diff>
--- a/Design Docs/STM32 Pin Allocation.xlsx
+++ b/Design Docs/STM32 Pin Allocation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B97A0-EE11-4B1C-9DED-E82C3A89A22B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C566DBE-1E2B-4CFB-99F2-BD5509D65BE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="354" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6435" yWindow="3120" windowWidth="14400" windowHeight="8273" tabRatio="354" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,266 +702,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1303,8 +1044,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="J28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1392,7 +1133,7 @@
         <v>89</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1438,7 +1179,7 @@
         <v>89</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1484,7 +1225,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1530,7 +1271,7 @@
         <v>89</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2151,7 +1892,7 @@
         <v>89</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
@@ -2197,7 +1938,7 @@
         <v>89</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
@@ -2243,7 +1984,7 @@
         <v>89</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
@@ -2312,7 +2053,7 @@
         <v>89</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -2381,7 +2122,7 @@
         <v>89</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
@@ -2941,7 +2682,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2967,7 +2708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2987,7 +2728,7 @@
         <v>70</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3107,29 +2848,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G39 P2:P39">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="(POWER)">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="(POWER)">
       <formula>NOT(ISERROR(SEARCH("(POWER)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="(CAN)">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="(CAN)">
       <formula>NOT(ISERROR(SEARCH("(CAN)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="(SPI)">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="(SPI)">
       <formula>NOT(ISERROR(SEARCH("(SPI)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="(ADC)">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="(ADC)">
       <formula>NOT(ISERROR(SEARCH("(ADC)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="18" priority="12">
+    <cfRule type="containsBlanks" dxfId="3" priority="12">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F39 K2:O39">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:P39">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="NC">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NC">
       <formula>NOT(ISERROR(SEARCH("NC",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>